<commit_message>
added control panel, added max lengths for long days
</commit_message>
<xml_diff>
--- a/iron_man_2025_training_plan.xlsx
+++ b/iron_man_2025_training_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9678D579B68F3777/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5E266D1-424E-47CE-9781-A8458BB656F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6609677E-A11D-4A26-9D08-DE2CF5310FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{38F0F4F5-960D-46EF-9A40-F4468FF4285D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" xr2:uid="{38F0F4F5-960D-46EF-9A40-F4468FF4285D}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
   <si>
     <t>Week
 (mon)</t>
@@ -134,12 +134,15 @@
     <t>Trun</t>
   </si>
   <si>
-    <t>weekly volume increase</t>
+    <t>Control Panel</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>Weekly Volume Increase</t>
+  </si>
+  <si>
     <t>Recovery week decrease relative to prior</t>
   </si>
   <si>
@@ -150,6 +153,15 @@
   </si>
   <si>
     <t>Daily max run</t>
+  </si>
+  <si>
+    <t>Long bike max</t>
+  </si>
+  <si>
+    <t>Long run max</t>
+  </si>
+  <si>
+    <t>Long swim max</t>
   </si>
   <si>
     <t>swim round(m)</t>
@@ -427,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -435,15 +447,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -468,6 +518,13 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -836,87 +893,87 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K19" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8:P32"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="13"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
-    <col min="17" max="19" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="12"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="17" max="19" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" ht="37.5">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:26" s="6" customFormat="1" ht="27">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="7" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="7" t="s">
+      <c r="T1" s="9"/>
+      <c r="U1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:26">
       <c r="A2" s="1">
         <v>45691</v>
       </c>
@@ -927,72 +984,81 @@
         <f t="shared" ref="C2:C30" si="0">C3+1</f>
         <v>30</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <f>1800</f>
         <v>1800</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <f>45</f>
         <v>45</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <f>3</f>
         <v>3</v>
       </c>
-      <c r="H2" s="11">
-        <f>MROUND(MIN($D2/3,$U$8),$U$12)</f>
+      <c r="H2" s="10">
+        <f>MROUND(MIN($D2/3,$Z$5),$Z$10)</f>
         <v>600</v>
       </c>
-      <c r="I2" s="11">
-        <f>MROUND(MIN($E2/3,$U$6),$U$14)</f>
+      <c r="I2" s="10">
+        <f>MROUND(MIN($E2/3,$Z$4),$Z$11)</f>
         <v>15</v>
       </c>
-      <c r="J2" s="11">
-        <f>MROUND(MIN($F2/3,$U$10),$U$16)</f>
+      <c r="J2" s="10">
+        <f>MROUND(MIN($F2/3,$Z$6),$Z$12)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="11">
-        <f>MROUND(MIN($D2/3,$U$8),$U$12)</f>
+      <c r="K2" s="10">
+        <f>MROUND(MIN($D2/3,$Z$5),$Z$10)</f>
         <v>600</v>
       </c>
-      <c r="L2" s="11">
-        <f>MROUND(MIN($E2/3,$U$6),$U$14)</f>
+      <c r="L2" s="10">
+        <f>MROUND(MIN($E2/3,$Z$4),$Z$11)</f>
         <v>15</v>
       </c>
-      <c r="M2" s="11">
-        <f>MROUND(MIN($F2/3,$U$10),$U$16)</f>
+      <c r="M2" s="10">
+        <f>MROUND(MIN($F2/3,$Z$6),$Z$12)</f>
         <v>1</v>
       </c>
-      <c r="N2" s="11">
-        <f>MROUND(D2-H2-K2,$U$12)</f>
+      <c r="N2" s="10">
+        <f>MIN(MROUND(D2-H2-K2,$Z$10),$Z$9)</f>
         <v>600</v>
       </c>
-      <c r="O2" s="11">
-        <f>MROUND(E2-I2-L2,$U$14)</f>
+      <c r="O2" s="10">
+        <f>MIN(MROUND(E2-I2-L2,$Z$11),$Z$7)</f>
         <v>15</v>
       </c>
-      <c r="P2" s="11">
-        <f>MROUND(F2-J2-M2,$U$16)</f>
+      <c r="P2" s="10">
+        <f>MIN(MROUND(F2-J2-M2,$Z$12),$Z$8)</f>
         <v>1</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <f>D2-H2-K2-N2</f>
         <v>0</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <f>E2-I2-L2-O2</f>
         <v>0</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <f>F2-J2-M2-P2</f>
         <v>0</v>
       </c>
-      <c r="T2" s="6"/>
-      <c r="U2" s="2">
+      <c r="T2" s="5"/>
+      <c r="U2" s="19">
+        <v>1</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="16">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
         <f>A2+7</f>
         <v>45698</v>
@@ -1004,72 +1070,81 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="D3" s="3" cm="1">
-        <f t="array" ref="D3">_xlfn.SWITCH($B3,"N",D2*(1+$U$2),"Y",D2*(1-$U$4))</f>
+      <c r="D3" s="2" cm="1">
+        <f t="array" ref="D3">_xlfn.SWITCH($B3,"N",D2*(1+$Z$2),"Y",D2*(1-$Z$3))</f>
         <v>1980.0000000000002</v>
       </c>
-      <c r="E3" s="3" cm="1">
-        <f t="array" ref="E3">_xlfn.SWITCH($B3,"N",E2*(1+$U$2),"Y",E2*(1-$U$4))</f>
+      <c r="E3" s="2" cm="1">
+        <f t="array" ref="E3">_xlfn.SWITCH($B3,"N",E2*(1+$Z$2),"Y",E2*(1-$Z$3))</f>
         <v>49.500000000000007</v>
       </c>
-      <c r="F3" s="13" cm="1">
-        <f t="array" ref="F3">_xlfn.SWITCH($B3,"N",F2*(1+$U$2),"Y",F2*(1-$U$4))</f>
+      <c r="F3" s="12" cm="1">
+        <f t="array" ref="F3">_xlfn.SWITCH($B3,"N",F2*(1+$Z$2),"Y",F2*(1-$Z$3))</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="H3" s="11">
-        <f>MROUND(MIN($D3/3,$U$8),$U$12)</f>
+      <c r="H3" s="10">
+        <f>MROUND(MIN($D3/3,$Z$5),$Z$10)</f>
         <v>650</v>
       </c>
-      <c r="I3" s="11">
-        <f>MROUND(MIN($E3/3,$U$6),$U$14)</f>
+      <c r="I3" s="10">
+        <f>MROUND(MIN($E3/3,$Z$4),$Z$11)</f>
         <v>17</v>
       </c>
-      <c r="J3" s="11">
-        <f>MROUND(MIN($F3/3,$U$10),$U$16)</f>
+      <c r="J3" s="10">
+        <f>MROUND(MIN($F3/3,$Z$6),$Z$12)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="K3" s="11">
-        <f>MROUND(MIN($D3/3,$U$8),$U$12)</f>
+      <c r="K3" s="10">
+        <f>MROUND(MIN($D3/3,$Z$5),$Z$10)</f>
         <v>650</v>
       </c>
-      <c r="L3" s="11">
-        <f>MROUND(MIN($E3/3,$U$6),$U$14)</f>
+      <c r="L3" s="10">
+        <f>MROUND(MIN($E3/3,$Z$4),$Z$11)</f>
         <v>17</v>
       </c>
-      <c r="M3" s="11">
-        <f>MROUND(MIN($F3/3,$U$10),$U$16)</f>
+      <c r="M3" s="10">
+        <f>MROUND(MIN($F3/3,$Z$6),$Z$12)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="N3" s="11">
-        <f t="shared" ref="N3:N32" si="1">MROUND(D3-H3-K3,$U$12)</f>
+      <c r="N3" s="10">
+        <f t="shared" ref="N3:N32" si="1">MIN(MROUND(D3-H3-K3,$Z$10),$Z$9)</f>
         <v>700</v>
       </c>
-      <c r="O3" s="11">
-        <f t="shared" ref="O3:O32" si="2">MROUND(E3-I3-L3,$U$14)</f>
+      <c r="O3" s="10">
+        <f t="shared" ref="O3:O32" si="2">MIN(MROUND(E3-I3-L3,$Z$11),$Z$7)</f>
         <v>16</v>
       </c>
-      <c r="P3" s="11">
-        <f t="shared" ref="P3:P32" si="3">MROUND(F3-J3-M3,$U$16)</f>
+      <c r="P3" s="10">
+        <f t="shared" ref="P3:P32" si="3">MIN(MROUND(F3-J3-M3,$Z$12),$Z$8)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="2">
         <f t="shared" ref="Q3:Q32" si="4">D3-H3-K3-N3</f>
         <v>-19.999999999999773</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="2">
         <f t="shared" ref="R3:R32" si="5">E3-I3-L3-O3</f>
         <v>-0.49999999999999289</v>
       </c>
-      <c r="S3" s="3">
+      <c r="S3" s="2">
         <f t="shared" ref="S3:S32" si="6">F3-J3-M3-P3</f>
         <v>0</v>
       </c>
-      <c r="T3" s="6"/>
-      <c r="U3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="T3" s="5"/>
+      <c r="U3" s="19">
+        <v>2</v>
+      </c>
+      <c r="V3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A32" si="7">A3+7</f>
         <v>45705</v>
@@ -1081,72 +1156,81 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="D4" s="3" cm="1">
-        <f t="array" ref="D4">_xlfn.SWITCH($B4,"N",D3*(1+$U$2),"Y",D3*(1-$U$4))</f>
+      <c r="D4" s="2" cm="1">
+        <f t="array" ref="D4">_xlfn.SWITCH($B4,"N",D3*(1+$Z$2),"Y",D3*(1-$Z$3))</f>
         <v>2178.0000000000005</v>
       </c>
-      <c r="E4" s="3" cm="1">
-        <f t="array" ref="E4">_xlfn.SWITCH($B4,"N",E3*(1+$U$2),"Y",E3*(1-$U$4))</f>
+      <c r="E4" s="2" cm="1">
+        <f t="array" ref="E4">_xlfn.SWITCH($B4,"N",E3*(1+$Z$2),"Y",E3*(1-$Z$3))</f>
         <v>54.45000000000001</v>
       </c>
-      <c r="F4" s="13" cm="1">
-        <f t="array" ref="F4">_xlfn.SWITCH($B4,"N",F3*(1+$U$2),"Y",F3*(1-$U$4))</f>
+      <c r="F4" s="12" cm="1">
+        <f t="array" ref="F4">_xlfn.SWITCH($B4,"N",F3*(1+$Z$2),"Y",F3*(1-$Z$3))</f>
         <v>3.6300000000000008</v>
       </c>
-      <c r="H4" s="11">
-        <f t="shared" ref="H4:H32" si="8">MROUND(MIN($D4/3,$U$8),$U$12)</f>
+      <c r="H4" s="10">
+        <f>MROUND(MIN($D4/3,$Z$5),$Z$10)</f>
         <v>750</v>
       </c>
-      <c r="I4" s="11">
-        <f t="shared" ref="I4:I32" si="9">MROUND(MIN($E4/3,$U$6),$U$14)</f>
+      <c r="I4" s="10">
+        <f>MROUND(MIN($E4/3,$Z$4),$Z$11)</f>
         <v>18</v>
       </c>
-      <c r="J4" s="11">
-        <f t="shared" ref="J4:J32" si="10">MROUND(MIN($F4/3,$U$10),$U$16)</f>
+      <c r="J4" s="10">
+        <f>MROUND(MIN($F4/3,$Z$6),$Z$12)</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="K4" s="11">
-        <f t="shared" ref="K4:K32" si="11">MROUND(MIN($D4/3,$U$8),$U$12)</f>
+      <c r="K4" s="10">
+        <f>MROUND(MIN($D4/3,$Z$5),$Z$10)</f>
         <v>750</v>
       </c>
-      <c r="L4" s="11">
-        <f t="shared" ref="L4:L32" si="12">MROUND(MIN($E4/3,$U$6),$U$14)</f>
+      <c r="L4" s="10">
+        <f>MROUND(MIN($E4/3,$Z$4),$Z$11)</f>
         <v>18</v>
       </c>
-      <c r="M4" s="11">
-        <f t="shared" ref="M4:M32" si="13">MROUND(MIN($F4/3,$U$10),$U$16)</f>
+      <c r="M4" s="10">
+        <f>MROUND(MIN($F4/3,$Z$6),$Z$12)</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="10">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <f t="shared" si="4"/>
         <v>-21.999999999999545</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="2">
         <f t="shared" si="5"/>
         <v>0.45000000000000995</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="2">
         <f t="shared" si="6"/>
         <v>3.0000000000000249E-2</v>
       </c>
-      <c r="T4" s="6"/>
-      <c r="U4" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="T4" s="5"/>
+      <c r="U4" s="19">
+        <v>3</v>
+      </c>
+      <c r="V4" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <f t="shared" si="7"/>
         <v>45712</v>
@@ -1158,72 +1242,81 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="D5" s="3" cm="1">
-        <f t="array" ref="D5">_xlfn.SWITCH($B5,"N",D4*(1+$U$2),"Y",D4*(1-$U$4))</f>
+      <c r="D5" s="2" cm="1">
+        <f t="array" ref="D5">_xlfn.SWITCH($B5,"N",D4*(1+$Z$2),"Y",D4*(1-$Z$3))</f>
         <v>2395.8000000000006</v>
       </c>
-      <c r="E5" s="3" cm="1">
-        <f t="array" ref="E5">_xlfn.SWITCH($B5,"N",E4*(1+$U$2),"Y",E4*(1-$U$4))</f>
+      <c r="E5" s="2" cm="1">
+        <f t="array" ref="E5">_xlfn.SWITCH($B5,"N",E4*(1+$Z$2),"Y",E4*(1-$Z$3))</f>
         <v>59.895000000000017</v>
       </c>
-      <c r="F5" s="13" cm="1">
-        <f t="array" ref="F5">_xlfn.SWITCH($B5,"N",F4*(1+$U$2),"Y",F4*(1-$U$4))</f>
+      <c r="F5" s="12" cm="1">
+        <f t="array" ref="F5">_xlfn.SWITCH($B5,"N",F4*(1+$Z$2),"Y",F4*(1-$Z$3))</f>
         <v>3.9930000000000012</v>
       </c>
-      <c r="H5" s="11">
-        <f t="shared" si="8"/>
+      <c r="H5" s="10">
+        <f>MROUND(MIN($D5/3,$Z$5),$Z$10)</f>
         <v>800</v>
       </c>
-      <c r="I5" s="11">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="10"/>
+      <c r="I5" s="10">
+        <f>MROUND(MIN($E5/3,$Z$4),$Z$11)</f>
+        <v>20</v>
+      </c>
+      <c r="J5" s="10">
+        <f>MROUND(MIN($F5/3,$Z$6),$Z$12)</f>
         <v>1.3</v>
       </c>
-      <c r="K5" s="11">
-        <f t="shared" si="11"/>
+      <c r="K5" s="10">
+        <f>MROUND(MIN($D5/3,$Z$5),$Z$10)</f>
         <v>800</v>
       </c>
-      <c r="L5" s="11">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="M5" s="11">
-        <f t="shared" si="13"/>
+      <c r="L5" s="10">
+        <f>MROUND(MIN($E5/3,$Z$4),$Z$11)</f>
+        <v>20</v>
+      </c>
+      <c r="M5" s="10">
+        <f>MROUND(MIN($F5/3,$Z$6),$Z$12)</f>
         <v>1.3</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="10">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="10">
         <f t="shared" si="3"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <f t="shared" si="4"/>
         <v>-4.1999999999993634</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="2">
         <f t="shared" si="5"/>
         <v>-0.10499999999998266</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="2">
         <f t="shared" si="6"/>
         <v>-6.999999999998785E-3</v>
       </c>
-      <c r="T5" s="6"/>
-      <c r="U5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="T5" s="5"/>
+      <c r="U5" s="19">
+        <v>4</v>
+      </c>
+      <c r="V5" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <f t="shared" si="7"/>
         <v>45719</v>
@@ -1235,71 +1328,80 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="D6" s="3" cm="1">
-        <f t="array" ref="D6">_xlfn.SWITCH($B6,"N",D5*(1+$U$2),"Y",D5*(1-$U$4))</f>
+      <c r="D6" s="2" cm="1">
+        <f t="array" ref="D6">_xlfn.SWITCH($B6,"N",D5*(1+$Z$2),"Y",D5*(1-$Z$3))</f>
         <v>2635.380000000001</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>60</v>
       </c>
-      <c r="F6" s="13" cm="1">
-        <f t="array" ref="F6">_xlfn.SWITCH($B6,"N",F5*(1+$U$2),"Y",F5*(1-$U$4))</f>
+      <c r="F6" s="12" cm="1">
+        <f t="array" ref="F6">_xlfn.SWITCH($B6,"N",F5*(1+$Z$2),"Y",F5*(1-$Z$3))</f>
         <v>4.3923000000000014</v>
       </c>
-      <c r="H6" s="11">
-        <f t="shared" si="8"/>
+      <c r="H6" s="10">
+        <f>MROUND(MIN($D6/3,$Z$5),$Z$10)</f>
         <v>900</v>
       </c>
-      <c r="I6" s="11">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="J6" s="11">
-        <f t="shared" si="10"/>
+      <c r="I6" s="10">
+        <f>MROUND(MIN($E6/3,$Z$4),$Z$11)</f>
+        <v>20</v>
+      </c>
+      <c r="J6" s="10">
+        <f>MROUND(MIN($F6/3,$Z$6),$Z$12)</f>
         <v>1.5</v>
       </c>
-      <c r="K6" s="11">
-        <f t="shared" si="11"/>
+      <c r="K6" s="10">
+        <f>MROUND(MIN($D6/3,$Z$5),$Z$10)</f>
         <v>900</v>
       </c>
-      <c r="L6" s="11">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="M6" s="11">
-        <f t="shared" si="13"/>
+      <c r="L6" s="10">
+        <f>MROUND(MIN($E6/3,$Z$4),$Z$11)</f>
+        <v>20</v>
+      </c>
+      <c r="M6" s="10">
+        <f>MROUND(MIN($F6/3,$Z$6),$Z$12)</f>
         <v>1.5</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="10">
         <f t="shared" si="1"/>
         <v>850</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="10">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="10">
         <f t="shared" si="3"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="2">
         <f t="shared" si="4"/>
         <v>-14.619999999998981</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="2">
         <f t="shared" si="6"/>
         <v>-7.6999999999987079E-3</v>
       </c>
-      <c r="T6" s="6"/>
-      <c r="U6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="T6" s="5"/>
+      <c r="U6" s="19">
+        <v>5</v>
+      </c>
+      <c r="V6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="1">
         <f t="shared" si="7"/>
         <v>45726</v>
@@ -1311,71 +1413,80 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="D7" s="3" cm="1">
-        <f t="array" ref="D7">_xlfn.SWITCH($B7,"N",D6*(1+$U$2),"Y",D6*(1-$U$4))</f>
+      <c r="D7" s="2" cm="1">
+        <f t="array" ref="D7">_xlfn.SWITCH($B7,"N",D6*(1+$Z$2),"Y",D6*(1-$Z$3))</f>
         <v>2898.9180000000015</v>
       </c>
-      <c r="E7" s="3" cm="1">
-        <f t="array" ref="E7">_xlfn.SWITCH($B7,"N",E6*(1+$U$2),"Y",E6*(1-$U$4))</f>
+      <c r="E7" s="2" cm="1">
+        <f t="array" ref="E7">_xlfn.SWITCH($B7,"N",E6*(1+$Z$2),"Y",E6*(1-$Z$3))</f>
         <v>66</v>
       </c>
-      <c r="F7" s="15">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11">
-        <f t="shared" si="8"/>
+      <c r="F7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <f>MROUND(MIN($D7/3,$Z$5),$Z$10)</f>
         <v>950</v>
       </c>
-      <c r="I7" s="11">
-        <f>MROUND(MIN($E7/3,$U$6),$U$14)</f>
-        <v>20</v>
-      </c>
-      <c r="J7" s="11">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="11">
-        <f t="shared" si="11"/>
+      <c r="I7" s="10">
+        <f>MROUND(MIN($E7/3,$Z$4),$Z$11)</f>
+        <v>20</v>
+      </c>
+      <c r="J7" s="10">
+        <f>MROUND(MIN($F7/3,$Z$6),$Z$12)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <f>MROUND(MIN($D7/3,$Z$5),$Z$10)</f>
         <v>950</v>
       </c>
-      <c r="L7" s="11">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="M7" s="11">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="11">
+      <c r="L7" s="10">
+        <f>MROUND(MIN($E7/3,$Z$4),$Z$11)</f>
+        <v>20</v>
+      </c>
+      <c r="M7" s="10">
+        <f>MROUND(MIN($F7/3,$Z$6),$Z$12)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="2">
         <f t="shared" si="4"/>
         <v>-1.0819999999985157</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T7" s="6"/>
-      <c r="U7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="T7" s="5"/>
+      <c r="U7" s="19">
+        <v>6</v>
+      </c>
+      <c r="V7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" s="1">
         <f t="shared" si="7"/>
         <v>45733</v>
@@ -1387,71 +1498,80 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D8" s="3" cm="1">
-        <f t="array" ref="D8">_xlfn.SWITCH($B8,"N",D7*(1+$U$2),"Y",D7*(1-$U$4))</f>
+      <c r="D8" s="2" cm="1">
+        <f t="array" ref="D8">_xlfn.SWITCH($B8,"N",D7*(1+$Z$2),"Y",D7*(1-$Z$3))</f>
         <v>3188.8098000000018</v>
       </c>
-      <c r="E8" s="3" cm="1">
-        <f t="array" ref="E8">_xlfn.SWITCH($B8,"N",E7*(1+$U$2),"Y",E7*(1-$U$4))</f>
+      <c r="E8" s="2" cm="1">
+        <f t="array" ref="E8">_xlfn.SWITCH($B8,"N",E7*(1+$Z$2),"Y",E7*(1-$Z$3))</f>
         <v>72.600000000000009</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D8/3,$Z$5),$Z$10)</f>
         <v>1050</v>
       </c>
       <c r="I8">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E8/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J8">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F8/3,$Z$6),$Z$12)</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D8/3,$Z$5),$Z$10)</f>
         <v>1050</v>
       </c>
       <c r="L8">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E8/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N8">
+        <f>MROUND(MIN($F8/3,$Z$6),$Z$12)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="20">
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="20">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="2">
         <f t="shared" si="4"/>
         <v>-11.190199999998185</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="2">
         <f t="shared" si="5"/>
         <v>-0.39999999999999147</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T8" s="6"/>
-      <c r="U8">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="T8" s="5"/>
+      <c r="U8" s="19">
+        <v>7</v>
+      </c>
+      <c r="V8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="1">
         <f t="shared" si="7"/>
         <v>45740</v>
@@ -1463,71 +1583,80 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D9" s="3" cm="1">
-        <f t="array" ref="D9">_xlfn.SWITCH($B9,"N",D8*(1+$U$2),"Y",D8*(1-$U$4))</f>
+      <c r="D9" s="2" cm="1">
+        <f t="array" ref="D9">_xlfn.SWITCH($B9,"N",D8*(1+$Z$2),"Y",D8*(1-$Z$3))</f>
         <v>3507.6907800000022</v>
       </c>
-      <c r="E9" s="3" cm="1">
-        <f t="array" ref="E9">_xlfn.SWITCH($B9,"N",E8*(1+$U$2),"Y",E8*(1-$U$4))</f>
+      <c r="E9" s="2" cm="1">
+        <f t="array" ref="E9">_xlfn.SWITCH($B9,"N",E8*(1+$Z$2),"Y",E8*(1-$Z$3))</f>
         <v>79.860000000000014</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D9/3,$Z$5),$Z$10)</f>
         <v>1150</v>
       </c>
       <c r="I9">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E9/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J9">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F9/3,$Z$6),$Z$12)</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D9/3,$Z$5),$Z$10)</f>
         <v>1150</v>
       </c>
       <c r="L9">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E9/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M9">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="N9">
+        <f>MROUND(MIN($F9/3,$Z$6),$Z$12)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="20">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="20">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <f t="shared" si="4"/>
         <v>7.690780000002178</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <f t="shared" si="5"/>
         <v>-0.13999999999998636</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T9" s="6"/>
-      <c r="U9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="T9" s="5"/>
+      <c r="U9" s="19">
+        <v>8</v>
+      </c>
+      <c r="V9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="1">
         <f t="shared" si="7"/>
         <v>45747</v>
@@ -1539,71 +1668,80 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D10" s="3" cm="1">
-        <f t="array" ref="D10">_xlfn.SWITCH($B10,"N",D9*(1+$U$2),"Y",D9*(1-$U$4))</f>
+      <c r="D10" s="2" cm="1">
+        <f t="array" ref="D10">_xlfn.SWITCH($B10,"N",D9*(1+$Z$2),"Y",D9*(1-$Z$3))</f>
         <v>3858.4598580000029</v>
       </c>
-      <c r="E10" s="3" cm="1">
-        <f t="array" ref="E10">_xlfn.SWITCH($B10,"N",E9*(1+$U$2),"Y",E9*(1-$U$4))</f>
+      <c r="E10" s="2" cm="1">
+        <f t="array" ref="E10">_xlfn.SWITCH($B10,"N",E9*(1+$Z$2),"Y",E9*(1-$Z$3))</f>
         <v>87.846000000000018</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>3</v>
       </c>
       <c r="H10">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D10/3,$Z$5),$Z$10)</f>
         <v>1300</v>
       </c>
       <c r="I10">
-        <f>MROUND(MIN($E10/3,$U$6),$U$14)</f>
+        <f>MROUND(MIN($E10/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J10">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F10/3,$Z$6),$Z$12)</f>
         <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D10/3,$Z$5),$Z$10)</f>
         <v>1300</v>
       </c>
       <c r="L10">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E10/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M10">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F10/3,$Z$6),$Z$12)</f>
         <v>1</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="20">
         <f t="shared" si="1"/>
         <v>1250</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="20">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="20">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10" s="2">
         <f t="shared" si="4"/>
         <v>8.459858000002896</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="2">
         <f t="shared" si="5"/>
         <v>-0.15399999999998215</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T10" s="6"/>
-      <c r="U10">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="T10" s="5"/>
+      <c r="U10" s="19">
+        <v>9</v>
+      </c>
+      <c r="V10" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="1">
         <f t="shared" si="7"/>
         <v>45754</v>
@@ -1615,72 +1753,81 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D11" s="3" cm="1">
-        <f t="array" ref="D11">_xlfn.SWITCH($B11,"N",D10*(1+$U$2),"Y",D10*(1-$U$4))</f>
+      <c r="D11" s="2" cm="1">
+        <f t="array" ref="D11">_xlfn.SWITCH($B11,"N",D10*(1+$Z$2),"Y",D10*(1-$Z$3))</f>
         <v>4244.3058438000035</v>
       </c>
-      <c r="E11" s="3" cm="1">
-        <f t="array" ref="E11">_xlfn.SWITCH($B11,"N",E10*(1+$U$2),"Y",E10*(1-$U$4))</f>
+      <c r="E11" s="2" cm="1">
+        <f t="array" ref="E11">_xlfn.SWITCH($B11,"N",E10*(1+$Z$2),"Y",E10*(1-$Z$3))</f>
         <v>96.63060000000003</v>
       </c>
-      <c r="F11" s="13" cm="1">
-        <f t="array" ref="F11">_xlfn.SWITCH($B11,"N",F10*(1+$U$2),"Y",F10*(1-$U$4))</f>
+      <c r="F11" s="12" cm="1">
+        <f t="array" ref="F11">_xlfn.SWITCH($B11,"N",F10*(1+$Z$2),"Y",F10*(1-$Z$3))</f>
         <v>3.3000000000000003</v>
       </c>
       <c r="H11">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D11/3,$Z$5),$Z$10)</f>
         <v>1400</v>
       </c>
       <c r="I11">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E11/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J11">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F11/3,$Z$6),$Z$12)</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K11">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D11/3,$Z$5),$Z$10)</f>
         <v>1400</v>
       </c>
       <c r="L11">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E11/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M11">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F11/3,$Z$6),$Z$12)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="N11">
-        <f>MROUND(D11-H11-K11,$U$12)</f>
+      <c r="N11" s="20">
+        <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="20">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="20">
         <f t="shared" si="3"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11" s="2">
         <f t="shared" si="4"/>
         <v>-5.6941561999965415</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11" s="2">
         <f t="shared" si="5"/>
         <v>-0.36939999999997042</v>
       </c>
-      <c r="S11" s="3">
+      <c r="S11" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T11" s="6"/>
-      <c r="U11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="T11" s="5"/>
+      <c r="U11" s="19">
+        <v>10</v>
+      </c>
+      <c r="V11" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="1">
         <f t="shared" si="7"/>
         <v>45761</v>
@@ -1692,72 +1839,81 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D12" s="3" cm="1">
-        <f t="array" ref="D12">_xlfn.SWITCH($B12,"N",D11*(1+$U$2),"Y",D11*(1-$U$4))</f>
+      <c r="D12" s="2" cm="1">
+        <f t="array" ref="D12">_xlfn.SWITCH($B12,"N",D11*(1+$Z$2),"Y",D11*(1-$Z$3))</f>
         <v>4668.7364281800046</v>
       </c>
-      <c r="E12" s="3" cm="1">
-        <f t="array" ref="E12">_xlfn.SWITCH($B12,"N",E11*(1+$U$2),"Y",E11*(1-$U$4))</f>
+      <c r="E12" s="2" cm="1">
+        <f t="array" ref="E12">_xlfn.SWITCH($B12,"N",E11*(1+$Z$2),"Y",E11*(1-$Z$3))</f>
         <v>106.29366000000005</v>
       </c>
-      <c r="F12" s="13" cm="1">
-        <f t="array" ref="F12">_xlfn.SWITCH($B12,"N",F11*(1+$U$2),"Y",F11*(1-$U$4))</f>
+      <c r="F12" s="12" cm="1">
+        <f t="array" ref="F12">_xlfn.SWITCH($B12,"N",F11*(1+$Z$2),"Y",F11*(1-$Z$3))</f>
         <v>3.6300000000000008</v>
       </c>
       <c r="H12">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D12/3,$Z$5),$Z$10)</f>
         <v>1550</v>
       </c>
       <c r="I12">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E12/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J12">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F12/3,$Z$6),$Z$12)</f>
         <v>1.2000000000000002</v>
       </c>
       <c r="K12">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D12/3,$Z$5),$Z$10)</f>
         <v>1550</v>
       </c>
       <c r="L12">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E12/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M12">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F12/3,$Z$6),$Z$12)</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="20">
         <f t="shared" si="1"/>
         <v>1550</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="20">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="20">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12" s="2">
         <f t="shared" si="4"/>
         <v>18.736428180004623</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="2">
         <f t="shared" si="5"/>
         <v>0.29366000000004533</v>
       </c>
-      <c r="S12" s="3">
+      <c r="S12" s="2">
         <f t="shared" si="6"/>
         <v>3.0000000000000249E-2</v>
       </c>
-      <c r="T12" s="6"/>
-      <c r="U12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="T12" s="5"/>
+      <c r="U12" s="19">
+        <v>11</v>
+      </c>
+      <c r="V12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="1">
         <f t="shared" si="7"/>
         <v>45768</v>
@@ -1769,72 +1925,82 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D13" s="3" cm="1">
-        <f t="array" ref="D13">_xlfn.SWITCH($B13,"N",D12*(1+$U$2),"Y",D12*(1-$U$4))</f>
+      <c r="D13" s="2" cm="1">
+        <f t="array" ref="D13">_xlfn.SWITCH($B13,"N",D12*(1+$Z$2),"Y",D12*(1-$Z$3))</f>
         <v>5135.6100709980055</v>
       </c>
-      <c r="E13" s="3" cm="1">
-        <f t="array" ref="E13">_xlfn.SWITCH($B13,"N",E12*(1+$U$2),"Y",E12*(1-$U$4))</f>
+      <c r="E13" s="2" cm="1">
+        <f t="array" ref="E13">_xlfn.SWITCH($B13,"N",E12*(1+$Z$2),"Y",E12*(1-$Z$3))</f>
         <v>116.92302600000006</v>
       </c>
-      <c r="F13" s="13" cm="1">
-        <f t="array" ref="F13">_xlfn.SWITCH($B13,"N",F12*(1+$U$2),"Y",F12*(1-$U$4))</f>
+      <c r="F13" s="12" cm="1">
+        <f t="array" ref="F13">_xlfn.SWITCH($B13,"N",F12*(1+$Z$2),"Y",F12*(1-$Z$3))</f>
         <v>3.9930000000000012</v>
       </c>
       <c r="H13">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D13/3,$Z$5),$Z$10)</f>
         <v>1700</v>
       </c>
       <c r="I13">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E13/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J13">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F13/3,$Z$6),$Z$12)</f>
         <v>1.3</v>
       </c>
       <c r="K13">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D13/3,$Z$5),$Z$10)</f>
         <v>1700</v>
       </c>
       <c r="L13">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E13/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M13">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F13/3,$Z$6),$Z$12)</f>
         <v>1.3</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="20">
         <f t="shared" si="1"/>
         <v>1750</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="20">
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="20">
         <f t="shared" si="3"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="2">
         <f t="shared" si="4"/>
         <v>-14.38992900199446</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="2">
         <f t="shared" si="5"/>
         <v>-7.6973999999935927E-2</v>
       </c>
-      <c r="S13" s="3">
+      <c r="S13" s="2">
         <f t="shared" si="6"/>
         <v>-6.999999999998785E-3</v>
       </c>
-      <c r="T13" s="6"/>
-      <c r="U13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="T13" s="5"/>
+      <c r="U13" s="19">
+        <v>12</v>
+      </c>
+      <c r="V13" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17" t="str" cm="1">
+        <f t="array" ref="Z13">IF(MAX(ABS(Q2:S32))&gt;50,"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" s="1">
         <f t="shared" si="7"/>
         <v>45775</v>
@@ -1846,72 +2012,69 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D14" s="3" cm="1">
-        <f t="array" ref="D14">_xlfn.SWITCH($B14,"N",D13*(1+$U$2),"Y",D13*(1-$U$4))</f>
+      <c r="D14" s="2" cm="1">
+        <f t="array" ref="D14">_xlfn.SWITCH($B14,"N",D13*(1+$Z$2),"Y",D13*(1-$Z$3))</f>
         <v>5649.1710780978065</v>
       </c>
-      <c r="E14" s="3" cm="1">
-        <f t="array" ref="E14">_xlfn.SWITCH($B14,"N",E13*(1+$U$2),"Y",E13*(1-$U$4))</f>
+      <c r="E14" s="2" cm="1">
+        <f t="array" ref="E14">_xlfn.SWITCH($B14,"N",E13*(1+$Z$2),"Y",E13*(1-$Z$3))</f>
         <v>128.61532860000008</v>
       </c>
-      <c r="F14" s="13" cm="1">
-        <f t="array" ref="F14">_xlfn.SWITCH($B14,"N",F13*(1+$U$2),"Y",F13*(1-$U$4))</f>
+      <c r="F14" s="12" cm="1">
+        <f t="array" ref="F14">_xlfn.SWITCH($B14,"N",F13*(1+$Z$2),"Y",F13*(1-$Z$3))</f>
         <v>4.3923000000000014</v>
       </c>
       <c r="H14">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D14/3,$Z$5),$Z$10)</f>
         <v>1900</v>
       </c>
       <c r="I14">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E14/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J14">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F14/3,$Z$6),$Z$12)</f>
         <v>1.5</v>
       </c>
       <c r="K14">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D14/3,$Z$5),$Z$10)</f>
         <v>1900</v>
       </c>
       <c r="L14">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E14/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M14">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F14/3,$Z$6),$Z$12)</f>
         <v>1.5</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="20">
         <f t="shared" si="1"/>
         <v>1850</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="20">
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="20">
         <f t="shared" si="3"/>
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="2">
         <f t="shared" si="4"/>
         <v>-0.82892190219354234</v>
       </c>
-      <c r="R14" s="3">
+      <c r="R14" s="2">
         <f t="shared" si="5"/>
         <v>-0.38467139999991673</v>
       </c>
-      <c r="S14" s="3">
+      <c r="S14" s="2">
         <f t="shared" si="6"/>
         <v>-7.6999999999987079E-3</v>
       </c>
-      <c r="T14" s="6"/>
-      <c r="U14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" s="1">
         <f t="shared" si="7"/>
         <v>45782</v>
@@ -1923,72 +2086,69 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D15" s="3" cm="1">
-        <f t="array" ref="D15">_xlfn.SWITCH($B15,"N",D14*(1+$U$2),"Y",D14*(1-$U$4))</f>
+      <c r="D15" s="2" cm="1">
+        <f t="array" ref="D15">_xlfn.SWITCH($B15,"N",D14*(1+$Z$2),"Y",D14*(1-$Z$3))</f>
         <v>6214.088185907588</v>
       </c>
-      <c r="E15" s="3" cm="1">
-        <f t="array" ref="E15">_xlfn.SWITCH($B15,"N",E14*(1+$U$2),"Y",E14*(1-$U$4))</f>
+      <c r="E15" s="2" cm="1">
+        <f t="array" ref="E15">_xlfn.SWITCH($B15,"N",E14*(1+$Z$2),"Y",E14*(1-$Z$3))</f>
         <v>141.47686146000009</v>
       </c>
-      <c r="F15" s="13" cm="1">
-        <f t="array" ref="F15">_xlfn.SWITCH($B15,"N",F14*(1+$U$2),"Y",F14*(1-$U$4))</f>
+      <c r="F15" s="12" cm="1">
+        <f t="array" ref="F15">_xlfn.SWITCH($B15,"N",F14*(1+$Z$2),"Y",F14*(1-$Z$3))</f>
         <v>4.8315300000000017</v>
       </c>
       <c r="H15">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D15/3,$Z$5),$Z$10)</f>
         <v>2050</v>
       </c>
       <c r="I15">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E15/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J15">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F15/3,$Z$6),$Z$12)</f>
         <v>1.6</v>
       </c>
       <c r="K15">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D15/3,$Z$5),$Z$10)</f>
         <v>2050</v>
       </c>
       <c r="L15">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E15/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M15">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F15/3,$Z$6),$Z$12)</f>
         <v>1.6</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="20">
         <f t="shared" si="1"/>
         <v>2100</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="20">
         <f t="shared" si="2"/>
         <v>101</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="20">
         <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="2">
         <f t="shared" si="4"/>
         <v>14.088185907588013</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="2">
         <f t="shared" si="5"/>
         <v>0.47686146000009444</v>
       </c>
-      <c r="S15" s="3">
+      <c r="S15" s="2">
         <f t="shared" si="6"/>
         <v>3.153000000000139E-2</v>
       </c>
-      <c r="T15" s="6"/>
-      <c r="U15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" s="1">
         <f t="shared" si="7"/>
         <v>45789</v>
@@ -2000,72 +2160,69 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D16" s="3" cm="1">
-        <f t="array" ref="D16">_xlfn.SWITCH($B16,"N",D15*(1+$U$2),"Y",D15*(1-$U$4))</f>
+      <c r="D16" s="2" cm="1">
+        <f t="array" ref="D16">_xlfn.SWITCH($B16,"N",D15*(1+$Z$2),"Y",D15*(1-$Z$3))</f>
         <v>6835.4970044983475</v>
       </c>
-      <c r="E16" s="3" cm="1">
-        <f t="array" ref="E16">_xlfn.SWITCH($B16,"N",E15*(1+$U$2),"Y",E15*(1-$U$4))</f>
+      <c r="E16" s="2" cm="1">
+        <f t="array" ref="E16">_xlfn.SWITCH($B16,"N",E15*(1+$Z$2),"Y",E15*(1-$Z$3))</f>
         <v>155.62454760600011</v>
       </c>
-      <c r="F16" s="13" cm="1">
-        <f t="array" ref="F16">_xlfn.SWITCH($B16,"N",F15*(1+$U$2),"Y",F15*(1-$U$4))</f>
+      <c r="F16" s="12" cm="1">
+        <f t="array" ref="F16">_xlfn.SWITCH($B16,"N",F15*(1+$Z$2),"Y",F15*(1-$Z$3))</f>
         <v>5.3146830000000023</v>
       </c>
       <c r="H16">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D16/3,$Z$5),$Z$10)</f>
         <v>2300</v>
       </c>
       <c r="I16">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E16/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J16">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F16/3,$Z$6),$Z$12)</f>
         <v>1.8</v>
       </c>
       <c r="K16">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D16/3,$Z$5),$Z$10)</f>
         <v>2300</v>
       </c>
       <c r="L16">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E16/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M16">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F16/3,$Z$6),$Z$12)</f>
         <v>1.8</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="20">
         <f t="shared" si="1"/>
         <v>2250</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="20">
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="20">
         <f t="shared" si="3"/>
         <v>1.7000000000000002</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16" s="2">
         <f t="shared" si="4"/>
         <v>-14.502995501652549</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16" s="2">
         <f t="shared" si="5"/>
         <v>-0.37545239399989327</v>
       </c>
-      <c r="S16" s="3">
+      <c r="S16" s="2">
         <f t="shared" si="6"/>
         <v>1.4683000000002222E-2</v>
       </c>
-      <c r="T16" s="6"/>
-      <c r="U16">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" s="1">
         <f t="shared" si="7"/>
         <v>45796</v>
@@ -2077,72 +2234,69 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D17" s="3" cm="1">
-        <f t="array" ref="D17">_xlfn.SWITCH($B17,"N",D16*(1+$U$2),"Y",D16*(1-$U$4))</f>
+      <c r="D17" s="2" cm="1">
+        <f t="array" ref="D17">_xlfn.SWITCH($B17,"N",D16*(1+$Z$2),"Y",D16*(1-$Z$3))</f>
         <v>7519.0467049481831</v>
       </c>
-      <c r="E17" s="3" cm="1">
-        <f t="array" ref="E17">_xlfn.SWITCH($B17,"N",E16*(1+$U$2),"Y",E16*(1-$U$4))</f>
+      <c r="E17" s="2" cm="1">
+        <f t="array" ref="E17">_xlfn.SWITCH($B17,"N",E16*(1+$Z$2),"Y",E16*(1-$Z$3))</f>
         <v>171.18700236660013</v>
       </c>
-      <c r="F17" s="13" cm="1">
-        <f t="array" ref="F17">_xlfn.SWITCH($B17,"N",F16*(1+$U$2),"Y",F16*(1-$U$4))</f>
+      <c r="F17" s="12" cm="1">
+        <f t="array" ref="F17">_xlfn.SWITCH($B17,"N",F16*(1+$Z$2),"Y",F16*(1-$Z$3))</f>
         <v>5.8461513000000034</v>
       </c>
       <c r="H17">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D17/3,$Z$5),$Z$10)</f>
         <v>2500</v>
       </c>
       <c r="I17">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E17/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J17">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F17/3,$Z$6),$Z$12)</f>
         <v>1.9000000000000001</v>
       </c>
       <c r="K17">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D17/3,$Z$5),$Z$10)</f>
         <v>2500</v>
       </c>
       <c r="L17">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E17/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M17">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F17/3,$Z$6),$Z$12)</f>
         <v>1.9000000000000001</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="20">
         <f t="shared" si="1"/>
         <v>2500</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="20">
         <f t="shared" si="2"/>
-        <v>131</v>
-      </c>
-      <c r="P17">
+        <v>120</v>
+      </c>
+      <c r="P17" s="20">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="Q17" s="2">
         <f t="shared" si="4"/>
         <v>19.046704948183105</v>
       </c>
-      <c r="R17" s="3">
+      <c r="R17" s="2">
         <f t="shared" si="5"/>
-        <v>0.18700236660012592</v>
-      </c>
-      <c r="S17" s="3">
+        <v>11.187002366600126</v>
+      </c>
+      <c r="S17" s="2">
         <f t="shared" si="6"/>
         <v>4.6151300000002671E-2</v>
       </c>
-      <c r="T17" s="6"/>
-      <c r="U17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" s="1">
         <f t="shared" si="7"/>
         <v>45803</v>
@@ -2154,73 +2308,69 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D18" s="3" cm="1">
-        <f t="array" ref="D18">_xlfn.SWITCH($B18,"N",D17*(1+$U$2),"Y",D17*(1-$U$4))</f>
+      <c r="D18" s="2" cm="1">
+        <f t="array" ref="D18">_xlfn.SWITCH($B18,"N",D17*(1+$Z$2),"Y",D17*(1-$Z$3))</f>
         <v>8270.9513754430027</v>
       </c>
-      <c r="E18" s="3" cm="1">
-        <f t="array" ref="E18">_xlfn.SWITCH($B18,"N",E17*(1+$U$2),"Y",E17*(1-$U$4))</f>
+      <c r="E18" s="2" cm="1">
+        <f t="array" ref="E18">_xlfn.SWITCH($B18,"N",E17*(1+$Z$2),"Y",E17*(1-$Z$3))</f>
         <v>188.30570260326016</v>
       </c>
-      <c r="F18" s="13" cm="1">
-        <f t="array" ref="F18">_xlfn.SWITCH($B18,"N",F17*(1+$U$2),"Y",F17*(1-$U$4))</f>
+      <c r="F18" s="12" cm="1">
+        <f t="array" ref="F18">_xlfn.SWITCH($B18,"N",F17*(1+$Z$2),"Y",F17*(1-$Z$3))</f>
         <v>6.4307664300000038</v>
       </c>
       <c r="H18">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D18/3,$Z$5),$Z$10)</f>
         <v>2750</v>
       </c>
       <c r="I18">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E18/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J18">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F18/3,$Z$6),$Z$12)</f>
         <v>2.1</v>
       </c>
       <c r="K18">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D18/3,$Z$5),$Z$10)</f>
         <v>2750</v>
       </c>
       <c r="L18">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E18/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M18">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F18/3,$Z$6),$Z$12)</f>
         <v>2.1</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="20">
         <f t="shared" si="1"/>
         <v>2750</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="20">
         <f t="shared" si="2"/>
-        <v>148</v>
-      </c>
-      <c r="P18">
+        <v>120</v>
+      </c>
+      <c r="P18" s="20">
         <f t="shared" si="3"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="Q18" s="2">
         <f t="shared" si="4"/>
         <v>20.951375443002689</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18" s="2">
         <f t="shared" si="5"/>
-        <v>0.30570260326015841</v>
-      </c>
-      <c r="S18" s="3">
+        <v>28.305702603260158</v>
+      </c>
+      <c r="S18" s="2">
         <f t="shared" si="6"/>
         <v>3.0766430000003897E-2</v>
       </c>
-      <c r="T18" s="6"/>
-      <c r="U18" t="str" cm="1">
-        <f t="array" ref="U18">IF(MAX(ABS(Q2:S32))&gt;50,"Yes","No")</f>
-        <v>No</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" s="1">
         <f t="shared" si="7"/>
         <v>45810</v>
@@ -2232,69 +2382,69 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D19" s="3" cm="1">
-        <f t="array" ref="D19">_xlfn.SWITCH($B19,"N",D18*(1+$U$2),"Y",D18*(1-$U$4))</f>
+      <c r="D19" s="2" cm="1">
+        <f t="array" ref="D19">_xlfn.SWITCH($B19,"N",D18*(1+$Z$2),"Y",D18*(1-$Z$3))</f>
         <v>9098.0465129873046</v>
       </c>
-      <c r="E19" s="3" cm="1">
-        <f t="array" ref="E19">_xlfn.SWITCH($B19,"N",E18*(1+$U$2),"Y",E18*(1-$U$4))</f>
+      <c r="E19" s="2" cm="1">
+        <f t="array" ref="E19">_xlfn.SWITCH($B19,"N",E18*(1+$Z$2),"Y",E18*(1-$Z$3))</f>
         <v>207.13627286358619</v>
       </c>
-      <c r="F19" s="13" cm="1">
-        <f t="array" ref="F19">_xlfn.SWITCH($B19,"N",F18*(1+$U$2),"Y",F18*(1-$U$4))</f>
+      <c r="F19" s="12" cm="1">
+        <f t="array" ref="F19">_xlfn.SWITCH($B19,"N",F18*(1+$Z$2),"Y",F18*(1-$Z$3))</f>
         <v>7.0738430730000044</v>
       </c>
       <c r="H19">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D19/3,$Z$5),$Z$10)</f>
         <v>3050</v>
       </c>
       <c r="I19">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E19/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J19">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F19/3,$Z$6),$Z$12)</f>
         <v>2.4000000000000004</v>
       </c>
       <c r="K19">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D19/3,$Z$5),$Z$10)</f>
         <v>3050</v>
       </c>
       <c r="L19">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E19/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M19">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F19/3,$Z$6),$Z$12)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="20">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="20">
         <f t="shared" si="2"/>
-        <v>167</v>
-      </c>
-      <c r="P19">
+        <v>120</v>
+      </c>
+      <c r="P19" s="20">
         <f t="shared" si="3"/>
         <v>2.3000000000000003</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="Q19" s="2">
         <f t="shared" si="4"/>
         <v>-1.9534870126954047</v>
       </c>
-      <c r="R19" s="3">
+      <c r="R19" s="2">
         <f t="shared" si="5"/>
-        <v>0.13627286358618562</v>
-      </c>
-      <c r="S19" s="3">
+        <v>47.136272863586186</v>
+      </c>
+      <c r="S19" s="2">
         <f t="shared" si="6"/>
         <v>-2.615692699999661E-2</v>
       </c>
-      <c r="T19" s="6"/>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" s="1">
         <f t="shared" si="7"/>
         <v>45817</v>
@@ -2306,69 +2456,69 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D20" s="3" cm="1">
-        <f t="array" ref="D20">_xlfn.SWITCH($B20,"N",D19*(1+$U$2),"Y",D19*(1-$U$4))</f>
+      <c r="D20" s="2" cm="1">
+        <f t="array" ref="D20">_xlfn.SWITCH($B20,"N",D19*(1+$Z$2),"Y",D19*(1-$Z$3))</f>
         <v>10007.851164286036</v>
       </c>
-      <c r="E20" s="3" cm="1">
-        <f t="array" ref="E20">_xlfn.SWITCH($B20,"N",E19*(1+$U$2),"Y",E19*(1-$U$4))</f>
+      <c r="E20" s="2" cm="1">
+        <f t="array" ref="E20">_xlfn.SWITCH($B20,"N",E19*(1+$Z$2),"Y",E19*(1-$Z$3))</f>
         <v>227.84990014994483</v>
       </c>
-      <c r="F20" s="13" cm="1">
-        <f t="array" ref="F20">_xlfn.SWITCH($B20,"N",F19*(1+$U$2),"Y",F19*(1-$U$4))</f>
+      <c r="F20" s="12" cm="1">
+        <f t="array" ref="F20">_xlfn.SWITCH($B20,"N",F19*(1+$Z$2),"Y",F19*(1-$Z$3))</f>
         <v>7.7812273803000052</v>
       </c>
       <c r="H20">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D20/3,$Z$5),$Z$10)</f>
         <v>3350</v>
       </c>
       <c r="I20">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E20/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J20">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F20/3,$Z$6),$Z$12)</f>
         <v>2.6</v>
       </c>
       <c r="K20">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D20/3,$Z$5),$Z$10)</f>
         <v>3350</v>
       </c>
       <c r="L20">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E20/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M20">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F20/3,$Z$6),$Z$12)</f>
         <v>2.6</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="20">
         <f t="shared" si="1"/>
         <v>3300</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="20">
         <f t="shared" si="2"/>
-        <v>188</v>
-      </c>
-      <c r="P20">
+        <v>120</v>
+      </c>
+      <c r="P20" s="20">
         <f t="shared" si="3"/>
         <v>2.6</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20" s="2">
         <f t="shared" si="4"/>
         <v>7.8511642860357824</v>
       </c>
-      <c r="R20" s="3">
+      <c r="R20" s="2">
         <f t="shared" si="5"/>
-        <v>-0.15009985005517024</v>
-      </c>
-      <c r="S20" s="3">
+        <v>67.84990014994483</v>
+      </c>
+      <c r="S20" s="2">
         <f t="shared" si="6"/>
         <v>-1.8772619699995552E-2</v>
       </c>
-      <c r="T20" s="6"/>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" s="1">
         <f t="shared" si="7"/>
         <v>45824</v>
@@ -2380,69 +2530,69 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D21" s="3" cm="1">
-        <f t="array" ref="D21">_xlfn.SWITCH($B21,"N",D20*(1+$U$2),"Y",D20*(1-$U$4))</f>
+      <c r="D21" s="2" cm="1">
+        <f t="array" ref="D21">_xlfn.SWITCH($B21,"N",D20*(1+$Z$2),"Y",D20*(1-$Z$3))</f>
         <v>11008.63628071464</v>
       </c>
-      <c r="E21" s="3" cm="1">
-        <f t="array" ref="E21">_xlfn.SWITCH($B21,"N",E20*(1+$U$2),"Y",E20*(1-$U$4))</f>
+      <c r="E21" s="2" cm="1">
+        <f t="array" ref="E21">_xlfn.SWITCH($B21,"N",E20*(1+$Z$2),"Y",E20*(1-$Z$3))</f>
         <v>250.63489016493932</v>
       </c>
-      <c r="F21" s="13" cm="1">
-        <f t="array" ref="F21">_xlfn.SWITCH($B21,"N",F20*(1+$U$2),"Y",F20*(1-$U$4))</f>
+      <c r="F21" s="12" cm="1">
+        <f t="array" ref="F21">_xlfn.SWITCH($B21,"N",F20*(1+$Z$2),"Y",F20*(1-$Z$3))</f>
         <v>8.5593501183300056</v>
       </c>
       <c r="H21">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D21/3,$Z$5),$Z$10)</f>
         <v>3650</v>
       </c>
       <c r="I21">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E21/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J21">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F21/3,$Z$6),$Z$12)</f>
         <v>2.9000000000000004</v>
       </c>
       <c r="K21">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D21/3,$Z$5),$Z$10)</f>
         <v>3650</v>
       </c>
       <c r="L21">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E21/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M21">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F21/3,$Z$6),$Z$12)</f>
         <v>2.9000000000000004</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="20">
         <f t="shared" si="1"/>
         <v>3700</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="20">
         <f t="shared" si="2"/>
-        <v>211</v>
-      </c>
-      <c r="P21">
+        <v>120</v>
+      </c>
+      <c r="P21" s="20">
         <f t="shared" si="3"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21" s="2">
         <f t="shared" si="4"/>
         <v>8.6362807146397245</v>
       </c>
-      <c r="R21" s="3">
+      <c r="R21" s="2">
         <f t="shared" si="5"/>
-        <v>-0.36510983506067873</v>
-      </c>
-      <c r="S21" s="3">
+        <v>90.634890164939321</v>
+      </c>
+      <c r="S21" s="2">
         <f t="shared" si="6"/>
         <v>-4.0649881669995391E-2</v>
       </c>
-      <c r="T21" s="6"/>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" s="1">
         <f t="shared" si="7"/>
         <v>45831</v>
@@ -2454,69 +2604,69 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D22" s="3" cm="1">
-        <f t="array" ref="D22">_xlfn.SWITCH($B22,"N",D21*(1+$U$2),"Y",D21*(1-$U$4))</f>
+      <c r="D22" s="2" cm="1">
+        <f t="array" ref="D22">_xlfn.SWITCH($B22,"N",D21*(1+$Z$2),"Y",D21*(1-$Z$3))</f>
         <v>12109.499908786105</v>
       </c>
-      <c r="E22" s="3" cm="1">
-        <f t="array" ref="E22">_xlfn.SWITCH($B22,"N",E21*(1+$U$2),"Y",E21*(1-$U$4))</f>
+      <c r="E22" s="2" cm="1">
+        <f t="array" ref="E22">_xlfn.SWITCH($B22,"N",E21*(1+$Z$2),"Y",E21*(1-$Z$3))</f>
         <v>275.69837918143327</v>
       </c>
-      <c r="F22" s="13" cm="1">
-        <f t="array" ref="F22">_xlfn.SWITCH($B22,"N",F21*(1+$U$2),"Y",F21*(1-$U$4))</f>
+      <c r="F22" s="12" cm="1">
+        <f t="array" ref="F22">_xlfn.SWITCH($B22,"N",F21*(1+$Z$2),"Y",F21*(1-$Z$3))</f>
         <v>9.4152851301630065</v>
       </c>
       <c r="H22">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D22/3,$Z$5),$Z$10)</f>
         <v>4050</v>
       </c>
       <c r="I22">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E22/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J22">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F22/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K22">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D22/3,$Z$5),$Z$10)</f>
         <v>4050</v>
       </c>
       <c r="L22">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E22/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M22">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F22/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="20">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="20">
         <f t="shared" si="2"/>
-        <v>236</v>
-      </c>
-      <c r="P22">
+        <v>120</v>
+      </c>
+      <c r="P22" s="20">
         <f t="shared" si="3"/>
         <v>3.2</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22" s="2">
         <f t="shared" si="4"/>
         <v>9.4999087861051521</v>
       </c>
-      <c r="R22" s="3">
+      <c r="R22" s="2">
         <f t="shared" si="5"/>
-        <v>-0.3016208185667324</v>
-      </c>
-      <c r="S22" s="3">
+        <v>115.69837918143327</v>
+      </c>
+      <c r="S22" s="2">
         <f t="shared" si="6"/>
         <v>1.5285130163006588E-2</v>
       </c>
-      <c r="T22" s="6"/>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23" s="1">
         <f t="shared" si="7"/>
         <v>45838</v>
@@ -2528,69 +2678,69 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D23" s="3" cm="1">
-        <f t="array" ref="D23">_xlfn.SWITCH($B23,"N",D22*(1+$U$2),"Y",D22*(1-$U$4))</f>
+      <c r="D23" s="2" cm="1">
+        <f t="array" ref="D23">_xlfn.SWITCH($B23,"N",D22*(1+$Z$2),"Y",D22*(1-$Z$3))</f>
         <v>13320.449899664716</v>
       </c>
-      <c r="E23" s="3" cm="1">
-        <f t="array" ref="E23">_xlfn.SWITCH($B23,"N",E22*(1+$U$2),"Y",E22*(1-$U$4))</f>
+      <c r="E23" s="2" cm="1">
+        <f t="array" ref="E23">_xlfn.SWITCH($B23,"N",E22*(1+$Z$2),"Y",E22*(1-$Z$3))</f>
         <v>303.26821709957665</v>
       </c>
-      <c r="F23" s="13" cm="1">
-        <f t="array" ref="F23">_xlfn.SWITCH($B23,"N",F22*(1+$U$2),"Y",F22*(1-$U$4))</f>
+      <c r="F23" s="12" cm="1">
+        <f t="array" ref="F23">_xlfn.SWITCH($B23,"N",F22*(1+$Z$2),"Y",F22*(1-$Z$3))</f>
         <v>10.356813643179308</v>
       </c>
       <c r="H23">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D23/3,$Z$5),$Z$10)</f>
         <v>4450</v>
       </c>
       <c r="I23">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E23/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J23">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F23/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K23">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D23/3,$Z$5),$Z$10)</f>
         <v>4450</v>
       </c>
       <c r="L23">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E23/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M23">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F23/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="20">
         <f t="shared" si="1"/>
         <v>4400</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="20">
         <f t="shared" si="2"/>
-        <v>263</v>
-      </c>
-      <c r="P23">
+        <v>120</v>
+      </c>
+      <c r="P23" s="20">
         <f t="shared" si="3"/>
         <v>4.2</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="Q23" s="2">
         <f t="shared" si="4"/>
         <v>20.449899664716213</v>
       </c>
-      <c r="R23" s="3">
+      <c r="R23" s="2">
         <f t="shared" si="5"/>
-        <v>0.26821709957664552</v>
-      </c>
-      <c r="S23" s="3">
+        <v>143.26821709957665</v>
+      </c>
+      <c r="S23" s="2">
         <f t="shared" si="6"/>
         <v>-4.3186356820691607E-2</v>
       </c>
-      <c r="T23" s="6"/>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" s="1">
         <f t="shared" si="7"/>
         <v>45845</v>
@@ -2602,69 +2752,69 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D24" s="3" cm="1">
-        <f t="array" ref="D24">_xlfn.SWITCH($B24,"N",D23*(1+$U$2),"Y",D23*(1-$U$4))</f>
+      <c r="D24" s="2" cm="1">
+        <f t="array" ref="D24">_xlfn.SWITCH($B24,"N",D23*(1+$Z$2),"Y",D23*(1-$Z$3))</f>
         <v>14652.494889631189</v>
       </c>
-      <c r="E24" s="3" cm="1">
-        <f t="array" ref="E24">_xlfn.SWITCH($B24,"N",E23*(1+$U$2),"Y",E23*(1-$U$4))</f>
+      <c r="E24" s="2" cm="1">
+        <f t="array" ref="E24">_xlfn.SWITCH($B24,"N",E23*(1+$Z$2),"Y",E23*(1-$Z$3))</f>
         <v>333.59503880953434</v>
       </c>
-      <c r="F24" s="13" cm="1">
-        <f t="array" ref="F24">_xlfn.SWITCH($B24,"N",F23*(1+$U$2),"Y",F23*(1-$U$4))</f>
+      <c r="F24" s="12" cm="1">
+        <f t="array" ref="F24">_xlfn.SWITCH($B24,"N",F23*(1+$Z$2),"Y",F23*(1-$Z$3))</f>
         <v>11.39249500749724</v>
       </c>
       <c r="H24">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D24/3,$Z$5),$Z$10)</f>
         <v>4900</v>
       </c>
       <c r="I24">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E24/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J24">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F24/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K24">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D24/3,$Z$5),$Z$10)</f>
         <v>4900</v>
       </c>
       <c r="L24">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E24/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M24">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F24/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="20">
         <f t="shared" si="1"/>
         <v>4850</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="20">
         <f t="shared" si="2"/>
-        <v>294</v>
-      </c>
-      <c r="P24">
+        <v>120</v>
+      </c>
+      <c r="P24" s="20">
         <f t="shared" si="3"/>
         <v>5.2</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24" s="2">
         <f t="shared" si="4"/>
         <v>2.4948896311889257</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24" s="2">
         <f t="shared" si="5"/>
-        <v>-0.40496119046565582</v>
-      </c>
-      <c r="S24" s="3">
+        <v>173.59503880953434</v>
+      </c>
+      <c r="S24" s="2">
         <f t="shared" si="6"/>
         <v>-7.5049925027590447E-3</v>
       </c>
-      <c r="T24" s="6"/>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" s="1">
         <f t="shared" si="7"/>
         <v>45852</v>
@@ -2676,69 +2826,69 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D25" s="3" cm="1">
-        <f t="array" ref="D25">_xlfn.SWITCH($B25,"N",D24*(1+$U$2),"Y",D24*(1-$U$4))</f>
+      <c r="D25" s="2" cm="1">
+        <f t="array" ref="D25">_xlfn.SWITCH($B25,"N",D24*(1+$Z$2),"Y",D24*(1-$Z$3))</f>
         <v>16117.744378594309</v>
       </c>
-      <c r="E25" s="3" cm="1">
-        <f t="array" ref="E25">_xlfn.SWITCH($B25,"N",E24*(1+$U$2),"Y",E24*(1-$U$4))</f>
+      <c r="E25" s="2" cm="1">
+        <f t="array" ref="E25">_xlfn.SWITCH($B25,"N",E24*(1+$Z$2),"Y",E24*(1-$Z$3))</f>
         <v>366.95454269048781</v>
       </c>
-      <c r="F25" s="13" cm="1">
-        <f t="array" ref="F25">_xlfn.SWITCH($B25,"N",F24*(1+$U$2),"Y",F24*(1-$U$4))</f>
+      <c r="F25" s="12" cm="1">
+        <f t="array" ref="F25">_xlfn.SWITCH($B25,"N",F24*(1+$Z$2),"Y",F24*(1-$Z$3))</f>
         <v>12.531744508246966</v>
       </c>
       <c r="H25">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D25/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I25">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E25/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J25">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F25/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K25">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D25/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L25">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E25/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M25">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F25/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="20">
         <f t="shared" si="1"/>
         <v>6100</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="20">
         <f t="shared" si="2"/>
-        <v>327</v>
-      </c>
-      <c r="P25">
+        <v>120</v>
+      </c>
+      <c r="P25" s="20">
         <f t="shared" si="3"/>
         <v>6.3000000000000007</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="Q25" s="2">
         <f t="shared" si="4"/>
         <v>17.744378594308728</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25" s="2">
         <f t="shared" si="5"/>
-        <v>-4.5457309512187294E-2</v>
-      </c>
-      <c r="S25" s="3">
+        <v>206.95454269048781</v>
+      </c>
+      <c r="S25" s="2">
         <f t="shared" si="6"/>
         <v>3.1744508246966063E-2</v>
       </c>
-      <c r="T25" s="6"/>
-    </row>
-    <row r="26" spans="1:21">
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" s="1">
         <f t="shared" si="7"/>
         <v>45859</v>
@@ -2750,69 +2900,69 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D26" s="3" cm="1">
-        <f t="array" ref="D26">_xlfn.SWITCH($B26,"N",D25*(1+$U$2),"Y",D25*(1-$U$4))</f>
+      <c r="D26" s="2" cm="1">
+        <f t="array" ref="D26">_xlfn.SWITCH($B26,"N",D25*(1+$Z$2),"Y",D25*(1-$Z$3))</f>
         <v>17729.518816453739</v>
       </c>
-      <c r="E26" s="3" cm="1">
-        <f t="array" ref="E26">_xlfn.SWITCH($B26,"N",E25*(1+$U$2),"Y",E25*(1-$U$4))</f>
+      <c r="E26" s="2" cm="1">
+        <f t="array" ref="E26">_xlfn.SWITCH($B26,"N",E25*(1+$Z$2),"Y",E25*(1-$Z$3))</f>
         <v>403.64999695953662</v>
       </c>
-      <c r="F26" s="13" cm="1">
-        <f t="array" ref="F26">_xlfn.SWITCH($B26,"N",F25*(1+$U$2),"Y",F25*(1-$U$4))</f>
+      <c r="F26" s="12" cm="1">
+        <f t="array" ref="F26">_xlfn.SWITCH($B26,"N",F25*(1+$Z$2),"Y",F25*(1-$Z$3))</f>
         <v>13.784918959071664</v>
       </c>
       <c r="H26">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D26/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I26">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E26/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J26">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F26/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K26">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D26/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L26">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E26/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M26">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F26/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="20">
         <f t="shared" si="1"/>
         <v>7750</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="20">
         <f t="shared" si="2"/>
-        <v>364</v>
-      </c>
-      <c r="P26">
+        <v>120</v>
+      </c>
+      <c r="P26" s="20">
         <f t="shared" si="3"/>
         <v>7.6000000000000005</v>
       </c>
-      <c r="Q26" s="3">
+      <c r="Q26" s="2">
         <f t="shared" si="4"/>
         <v>-20.481183546260581</v>
       </c>
-      <c r="R26" s="3">
+      <c r="R26" s="2">
         <f t="shared" si="5"/>
-        <v>-0.3500030404633776</v>
-      </c>
-      <c r="S26" s="3">
+        <v>243.64999695953662</v>
+      </c>
+      <c r="S26" s="2">
         <f t="shared" si="6"/>
         <v>-1.5081040928335732E-2</v>
       </c>
-      <c r="T26" s="6"/>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="1">
         <f t="shared" si="7"/>
         <v>45866</v>
@@ -2824,69 +2974,69 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D27" s="3" cm="1">
-        <f t="array" ref="D27">_xlfn.SWITCH($B27,"N",D26*(1+$U$2),"Y",D26*(1-$U$4))</f>
+      <c r="D27" s="2" cm="1">
+        <f t="array" ref="D27">_xlfn.SWITCH($B27,"N",D26*(1+$Z$2),"Y",D26*(1-$Z$3))</f>
         <v>19502.470698099114</v>
       </c>
-      <c r="E27" s="3" cm="1">
-        <f t="array" ref="E27">_xlfn.SWITCH($B27,"N",E26*(1+$U$2),"Y",E26*(1-$U$4))</f>
+      <c r="E27" s="2" cm="1">
+        <f t="array" ref="E27">_xlfn.SWITCH($B27,"N",E26*(1+$Z$2),"Y",E26*(1-$Z$3))</f>
         <v>444.01499665549034</v>
       </c>
-      <c r="F27" s="13" cm="1">
-        <f t="array" ref="F27">_xlfn.SWITCH($B27,"N",F26*(1+$U$2),"Y",F26*(1-$U$4))</f>
+      <c r="F27" s="12" cm="1">
+        <f t="array" ref="F27">_xlfn.SWITCH($B27,"N",F26*(1+$Z$2),"Y",F26*(1-$Z$3))</f>
         <v>15.163410854978832</v>
       </c>
       <c r="H27">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D27/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I27">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E27/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J27">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F27/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K27">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D27/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L27">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E27/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M27">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F27/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="20">
         <f t="shared" si="1"/>
         <v>9500</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="20">
         <f t="shared" si="2"/>
-        <v>404</v>
-      </c>
-      <c r="P27">
+        <v>120</v>
+      </c>
+      <c r="P27" s="20">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27" s="2">
         <f t="shared" si="4"/>
         <v>2.4706980991140881</v>
       </c>
-      <c r="R27" s="3">
+      <c r="R27" s="2">
         <f t="shared" si="5"/>
-        <v>1.4996655490335797E-2</v>
-      </c>
-      <c r="S27" s="3">
+        <v>284.01499665549034</v>
+      </c>
+      <c r="S27" s="2">
         <f t="shared" si="6"/>
         <v>-3.6589145021167724E-2</v>
       </c>
-      <c r="T27" s="6"/>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="T27" s="5"/>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="1">
         <f t="shared" si="7"/>
         <v>45873</v>
@@ -2898,69 +3048,69 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D28" s="3" cm="1">
-        <f t="array" ref="D28">_xlfn.SWITCH($B28,"N",D27*(1+$U$2),"Y",D27*(1-$U$4))</f>
+      <c r="D28" s="2" cm="1">
+        <f t="array" ref="D28">_xlfn.SWITCH($B28,"N",D27*(1+$Z$2),"Y",D27*(1-$Z$3))</f>
         <v>21452.717767909027</v>
       </c>
-      <c r="E28" s="3" cm="1">
-        <f t="array" ref="E28">_xlfn.SWITCH($B28,"N",E27*(1+$U$2),"Y",E27*(1-$U$4))</f>
+      <c r="E28" s="2" cm="1">
+        <f t="array" ref="E28">_xlfn.SWITCH($B28,"N",E27*(1+$Z$2),"Y",E27*(1-$Z$3))</f>
         <v>488.4164963210394</v>
       </c>
-      <c r="F28" s="13" cm="1">
-        <f t="array" ref="F28">_xlfn.SWITCH($B28,"N",F27*(1+$U$2),"Y",F27*(1-$U$4))</f>
+      <c r="F28" s="12" cm="1">
+        <f t="array" ref="F28">_xlfn.SWITCH($B28,"N",F27*(1+$Z$2),"Y",F27*(1-$Z$3))</f>
         <v>16.679751940476716</v>
       </c>
       <c r="H28">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D28/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I28">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E28/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J28">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F28/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K28">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D28/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L28">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E28/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M28">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F28/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="20">
         <f t="shared" si="1"/>
-        <v>11450</v>
-      </c>
-      <c r="O28">
+        <v>10000</v>
+      </c>
+      <c r="O28" s="20">
         <f t="shared" si="2"/>
-        <v>448</v>
-      </c>
-      <c r="P28">
+        <v>120</v>
+      </c>
+      <c r="P28" s="20">
         <f t="shared" si="3"/>
         <v>10.5</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28" s="2">
         <f t="shared" si="4"/>
-        <v>2.7177679090273159</v>
-      </c>
-      <c r="R28" s="3">
+        <v>1452.7177679090273</v>
+      </c>
+      <c r="R28" s="2">
         <f t="shared" si="5"/>
-        <v>0.41649632103940348</v>
-      </c>
-      <c r="S28" s="3">
+        <v>328.4164963210394</v>
+      </c>
+      <c r="S28" s="2">
         <f t="shared" si="6"/>
         <v>-2.0248059523282791E-2</v>
       </c>
-      <c r="T28" s="6"/>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="T28" s="5"/>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" s="1">
         <f t="shared" si="7"/>
         <v>45880</v>
@@ -2972,69 +3122,69 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D29" s="3" cm="1">
-        <f t="array" ref="D29">_xlfn.SWITCH($B29,"N",D28*(1+$U$2),"Y",D28*(1-$U$4))</f>
+      <c r="D29" s="2" cm="1">
+        <f t="array" ref="D29">_xlfn.SWITCH($B29,"N",D28*(1+$Z$2),"Y",D28*(1-$Z$3))</f>
         <v>23597.989544699933</v>
       </c>
-      <c r="E29" s="3" cm="1">
-        <f t="array" ref="E29">_xlfn.SWITCH($B29,"N",E28*(1+$U$2),"Y",E28*(1-$U$4))</f>
+      <c r="E29" s="2" cm="1">
+        <f t="array" ref="E29">_xlfn.SWITCH($B29,"N",E28*(1+$Z$2),"Y",E28*(1-$Z$3))</f>
         <v>537.25814595314341</v>
       </c>
-      <c r="F29" s="13" cm="1">
-        <f t="array" ref="F29">_xlfn.SWITCH($B29,"N",F28*(1+$U$2),"Y",F28*(1-$U$4))</f>
+      <c r="F29" s="12" cm="1">
+        <f t="array" ref="F29">_xlfn.SWITCH($B29,"N",F28*(1+$Z$2),"Y",F28*(1-$Z$3))</f>
         <v>18.347727134524391</v>
       </c>
       <c r="H29">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D29/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I29">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E29/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J29">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F29/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D29/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L29">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E29/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M29">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F29/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="20">
         <f t="shared" si="1"/>
-        <v>13600</v>
-      </c>
-      <c r="O29">
+        <v>10000</v>
+      </c>
+      <c r="O29" s="20">
         <f t="shared" si="2"/>
-        <v>497</v>
-      </c>
-      <c r="P29">
+        <v>120</v>
+      </c>
+      <c r="P29" s="20">
         <f t="shared" si="3"/>
         <v>12.100000000000001</v>
       </c>
-      <c r="Q29" s="3">
+      <c r="Q29" s="2">
         <f t="shared" si="4"/>
-        <v>-2.0104553000674059</v>
-      </c>
-      <c r="R29" s="3">
+        <v>3597.9895446999326</v>
+      </c>
+      <c r="R29" s="2">
         <f t="shared" si="5"/>
-        <v>0.25814595314341204</v>
-      </c>
-      <c r="S29" s="3">
+        <v>377.25814595314341</v>
+      </c>
+      <c r="S29" s="2">
         <f t="shared" si="6"/>
         <v>4.7727134524389925E-2</v>
       </c>
-      <c r="T29" s="6"/>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="1">
         <f t="shared" si="7"/>
         <v>45887</v>
@@ -3046,69 +3196,69 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D30" s="3" cm="1">
-        <f t="array" ref="D30">_xlfn.SWITCH($B30,"N",D29*(1+$U$2),"Y",D29*(1-$U$4))</f>
+      <c r="D30" s="2" cm="1">
+        <f t="array" ref="D30">_xlfn.SWITCH($B30,"N",D29*(1+$Z$2),"Y",D29*(1-$Z$3))</f>
         <v>25957.788499169928</v>
       </c>
-      <c r="E30" s="3" cm="1">
-        <f t="array" ref="E30">_xlfn.SWITCH($B30,"N",E29*(1+$U$2),"Y",E29*(1-$U$4))</f>
+      <c r="E30" s="2" cm="1">
+        <f t="array" ref="E30">_xlfn.SWITCH($B30,"N",E29*(1+$Z$2),"Y",E29*(1-$Z$3))</f>
         <v>590.98396054845784</v>
       </c>
-      <c r="F30" s="13" cm="1">
-        <f t="array" ref="F30">_xlfn.SWITCH($B30,"N",F29*(1+$U$2),"Y",F29*(1-$U$4))</f>
+      <c r="F30" s="12" cm="1">
+        <f t="array" ref="F30">_xlfn.SWITCH($B30,"N",F29*(1+$Z$2),"Y",F29*(1-$Z$3))</f>
         <v>20.182499847976832</v>
       </c>
       <c r="H30">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D30/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I30">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E30/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J30">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F30/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K30">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D30/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L30">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E30/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M30">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F30/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="20">
         <f t="shared" si="1"/>
-        <v>15950</v>
-      </c>
-      <c r="O30">
+        <v>10000</v>
+      </c>
+      <c r="O30" s="20">
         <f t="shared" si="2"/>
-        <v>551</v>
-      </c>
-      <c r="P30">
+        <v>120</v>
+      </c>
+      <c r="P30" s="20">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q30" s="2">
         <f t="shared" si="4"/>
-        <v>7.7884991699284001</v>
-      </c>
-      <c r="R30" s="3">
+        <v>5957.7884991699284</v>
+      </c>
+      <c r="R30" s="2">
         <f t="shared" si="5"/>
-        <v>-1.6039451542155803E-2</v>
-      </c>
-      <c r="S30" s="3">
+        <v>430.98396054845784</v>
+      </c>
+      <c r="S30" s="2">
         <f t="shared" si="6"/>
         <v>-1.7500152023169235E-2</v>
       </c>
-      <c r="T30" s="6"/>
-    </row>
-    <row r="31" spans="1:21">
+      <c r="T30" s="5"/>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="1">
         <f t="shared" si="7"/>
         <v>45894</v>
@@ -3120,69 +3270,69 @@
         <f>C32+1</f>
         <v>1</v>
       </c>
-      <c r="D31" s="3" cm="1">
-        <f t="array" ref="D31">_xlfn.SWITCH($B31,"N",D30*(1+$U$2),"Y",D30*(1-$U$4))</f>
+      <c r="D31" s="2" cm="1">
+        <f t="array" ref="D31">_xlfn.SWITCH($B31,"N",D30*(1+$Z$2),"Y",D30*(1-$Z$3))</f>
         <v>28553.567349086923</v>
       </c>
-      <c r="E31" s="3" cm="1">
-        <f t="array" ref="E31">_xlfn.SWITCH($B31,"N",E30*(1+$U$2),"Y",E30*(1-$U$4))</f>
+      <c r="E31" s="2" cm="1">
+        <f t="array" ref="E31">_xlfn.SWITCH($B31,"N",E30*(1+$Z$2),"Y",E30*(1-$Z$3))</f>
         <v>650.08235660330365</v>
       </c>
-      <c r="F31" s="13" cm="1">
-        <f t="array" ref="F31">_xlfn.SWITCH($B31,"N",F30*(1+$U$2),"Y",F30*(1-$U$4))</f>
+      <c r="F31" s="12" cm="1">
+        <f t="array" ref="F31">_xlfn.SWITCH($B31,"N",F30*(1+$Z$2),"Y",F30*(1-$Z$3))</f>
         <v>22.200749832774516</v>
       </c>
       <c r="H31">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D31/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I31">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E31/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J31">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F31/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K31">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D31/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L31">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E31/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M31">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F31/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="20">
         <f t="shared" si="1"/>
-        <v>18550</v>
-      </c>
-      <c r="O31">
+        <v>10000</v>
+      </c>
+      <c r="O31" s="20">
         <f t="shared" si="2"/>
-        <v>610</v>
-      </c>
-      <c r="P31">
+        <v>120</v>
+      </c>
+      <c r="P31" s="20">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q31" s="2">
         <f t="shared" si="4"/>
-        <v>3.5673490869230591</v>
-      </c>
-      <c r="R31" s="3">
+        <v>8553.5673490869231</v>
+      </c>
+      <c r="R31" s="2">
         <f t="shared" si="5"/>
-        <v>8.2356603303651355E-2</v>
-      </c>
-      <c r="S31" s="3">
+        <v>490.08235660330365</v>
+      </c>
+      <c r="S31" s="2">
         <f t="shared" si="6"/>
         <v>7.4983277451323715E-4</v>
       </c>
-      <c r="T31" s="6"/>
-    </row>
-    <row r="32" spans="1:21">
+      <c r="T31" s="5"/>
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" s="1">
         <f t="shared" si="7"/>
         <v>45901</v>
@@ -3193,67 +3343,67 @@
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32" s="3" cm="1">
-        <f t="array" ref="D32">_xlfn.SWITCH($B32,"N",D31*(1+$U$2),"Y",D31*(1-$U$4))</f>
+      <c r="D32" s="2" cm="1">
+        <f t="array" ref="D32">_xlfn.SWITCH($B32,"N",D31*(1+$Z$2),"Y",D31*(1-$Z$3))</f>
         <v>31408.924083995618</v>
       </c>
-      <c r="E32" s="3" cm="1">
-        <f t="array" ref="E32">_xlfn.SWITCH($B32,"N",E31*(1+$U$2),"Y",E31*(1-$U$4))</f>
+      <c r="E32" s="2" cm="1">
+        <f t="array" ref="E32">_xlfn.SWITCH($B32,"N",E31*(1+$Z$2),"Y",E31*(1-$Z$3))</f>
         <v>715.09059226363411</v>
       </c>
-      <c r="F32" s="13" cm="1">
-        <f t="array" ref="F32">_xlfn.SWITCH($B32,"N",F31*(1+$U$2),"Y",F31*(1-$U$4))</f>
+      <c r="F32" s="12" cm="1">
+        <f t="array" ref="F32">_xlfn.SWITCH($B32,"N",F31*(1+$Z$2),"Y",F31*(1-$Z$3))</f>
         <v>24.420824816051969</v>
       </c>
       <c r="H32">
-        <f t="shared" si="8"/>
+        <f>MROUND(MIN($D32/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="I32">
-        <f t="shared" si="9"/>
+        <f>MROUND(MIN($E32/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="J32">
-        <f t="shared" si="10"/>
+        <f>MROUND(MIN($F32/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
       <c r="K32">
-        <f t="shared" si="11"/>
+        <f>MROUND(MIN($D32/3,$Z$5),$Z$10)</f>
         <v>5000</v>
       </c>
       <c r="L32">
-        <f t="shared" si="12"/>
+        <f>MROUND(MIN($E32/3,$Z$4),$Z$11)</f>
         <v>20</v>
       </c>
       <c r="M32">
-        <f t="shared" si="13"/>
+        <f>MROUND(MIN($F32/3,$Z$6),$Z$12)</f>
         <v>3.1</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="20">
         <f t="shared" si="1"/>
-        <v>21400</v>
-      </c>
-      <c r="O32">
+        <v>10000</v>
+      </c>
+      <c r="O32" s="20">
         <f t="shared" si="2"/>
-        <v>675</v>
-      </c>
-      <c r="P32">
+        <v>120</v>
+      </c>
+      <c r="P32" s="20">
         <f t="shared" si="3"/>
         <v>18.2</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="Q32" s="2">
         <f t="shared" si="4"/>
-        <v>8.9240839956182754</v>
-      </c>
-      <c r="R32" s="3">
+        <v>11408.924083995618</v>
+      </c>
+      <c r="R32" s="2">
         <f t="shared" si="5"/>
-        <v>9.0592263634107439E-2</v>
-      </c>
-      <c r="S32" s="3">
+        <v>555.09059226363411</v>
+      </c>
+      <c r="S32" s="2">
         <f t="shared" si="6"/>
         <v>2.0824816051966621E-2</v>
       </c>
-      <c r="T32" s="6"/>
+      <c r="T32" s="5"/>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1"/>
@@ -3286,8 +3436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EBC209-BAD1-4137-B010-AA145F63AA9D}">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3304,75 +3454,75 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="N1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="O1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="P1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="Q1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="R1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="S1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F2">
         <v>6</v>
@@ -3390,7 +3540,7 @@
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L2">
         <v>140</v>
@@ -3405,21 +3555,21 @@
         <v>7</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -3437,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L3">
         <v>140</v>
@@ -3452,26 +3602,26 @@
         <v>6</v>
       </c>
       <c r="P3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="15"/>
       <c r="H4">
         <v>0</v>
       </c>
@@ -3482,7 +3632,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L4">
         <v>140</v>
@@ -3497,26 +3647,26 @@
         <v>6</v>
       </c>
       <c r="P4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>7</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="15"/>
       <c r="H5">
         <v>0</v>
       </c>
@@ -3527,7 +3677,7 @@
         <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L5">
         <v>150</v>
@@ -3542,26 +3692,26 @@
         <v>8</v>
       </c>
       <c r="P5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>10</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="15"/>
       <c r="H6">
         <v>0</v>
       </c>
@@ -3572,7 +3722,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L6">
         <v>150</v>
@@ -3587,26 +3737,26 @@
         <v>7</v>
       </c>
       <c r="P6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F7">
         <v>10</v>
       </c>
-      <c r="G7" s="16"/>
+      <c r="G7" s="15"/>
       <c r="H7">
         <v>100</v>
       </c>
@@ -3617,7 +3767,7 @@
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L7">
         <v>210</v>
@@ -3632,26 +3782,26 @@
         <v>11</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F8">
         <v>19</v>
       </c>
-      <c r="G8" s="16"/>
+      <c r="G8" s="15"/>
       <c r="H8">
         <v>0</v>
       </c>
@@ -3662,7 +3812,7 @@
         <v>11</v>
       </c>
       <c r="K8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L8">
         <v>400</v>
@@ -3677,26 +3827,26 @@
         <v>22</v>
       </c>
       <c r="P8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F9">
         <v>28</v>
       </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="15"/>
       <c r="H9">
         <v>50</v>
       </c>
@@ -3707,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L9">
         <v>160</v>
@@ -3722,26 +3872,26 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F10">
         <v>27</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="15"/>
       <c r="H10">
         <v>0</v>
       </c>
@@ -3752,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L10">
         <v>160</v>
@@ -3767,26 +3917,26 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F11">
         <v>16</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="15"/>
       <c r="H11">
         <v>25</v>
       </c>
@@ -3797,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L11">
         <v>70</v>
@@ -3812,26 +3962,26 @@
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="15"/>
       <c r="H12">
         <v>0</v>
       </c>
@@ -3842,7 +3992,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L12">
         <v>100</v>
@@ -3857,26 +4007,26 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F13">
         <v>11</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="15"/>
       <c r="H13">
         <v>32</v>
       </c>
@@ -3887,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L13">
         <v>100</v>
@@ -3902,26 +4052,26 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
         <v>88</v>
       </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F14">
         <v>16</v>
       </c>
-      <c r="G14" s="16"/>
+      <c r="G14" s="15"/>
       <c r="H14">
         <v>0</v>
       </c>
@@ -3932,7 +4082,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L14">
         <v>80</v>
@@ -3947,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>